<commit_message>
talk to Ali-Mohamadi tomorrow :wink:
</commit_message>
<xml_diff>
--- a/Data/Connections.xlsx
+++ b/Data/Connections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115B043F-2CCE-449A-9856-38E5E7E9883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6F053C-E916-4A8F-B3D4-679F6E459461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +121,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -237,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,9 +249,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,7 +540,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,22 +574,24 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>8855</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7">
+        <v>395246111</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>

</xml_diff>